<commit_message>
include scales and derivations
</commit_message>
<xml_diff>
--- a/data/predictions/preds_answerFromTable_mcot.xlsx
+++ b/data/predictions/preds_answerFromTable_mcot.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
           <t>label</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>scale</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>derivation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +476,12 @@
           <t>['146']</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,6 +503,16 @@
       <c r="C3" t="n">
         <v>3980.6</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>1,536.7+1,378.2+1,065.7</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -504,6 +530,8 @@
           <t>['Operating profit', 'Adjustments']</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -523,6 +551,12 @@
       </c>
       <c r="C5" t="n">
         <v>0.96</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">109.7/(0.41*278.29) </t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -551,6 +585,16 @@
       <c r="C6" t="n">
         <v>-0.05</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>(51.2/157.4)-(51.5/158.1)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -567,6 +611,16 @@
       </c>
       <c r="C7" t="n">
         <v>51.49</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>($3,341/$6,489)</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -588,6 +642,16 @@
       <c r="C8" t="n">
         <v>149.68</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(1,930 - 773)/773 </t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -605,6 +669,8 @@
           <t>['May']</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -619,6 +685,16 @@
       </c>
       <c r="C10" t="n">
         <v>4.9</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>51.3-46.4</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -638,6 +714,16 @@
       </c>
       <c r="C11" t="n">
         <v>1162802.5</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>(1,203,980 + 1,121,625) / 2</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -659,6 +745,16 @@
       <c r="C12" t="n">
         <v>972</v>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4,674 - 3,702 </t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -677,6 +773,16 @@
       <c r="C13" t="n">
         <v>6.98</v>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$124,665/$1,786,362</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -694,6 +800,12 @@
           <t>['(1,591)', '1,007']</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -714,6 +826,16 @@
       <c r="C15" t="n">
         <v>53.73</v>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$7,462/$13,889 </t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -729,6 +851,12 @@
       <c r="C16" t="inlineStr">
         <is>
           <t>['2018']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>locate and analyze Total operating expenses in row 10</t>
         </is>
       </c>
     </row>
@@ -750,6 +878,16 @@
       <c r="C17" t="n">
         <v>7634.33</v>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>(6,199+3,820+12,884) / 3</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -767,6 +905,12 @@
           <t>['$8,320', '$12,472']</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -784,6 +928,12 @@
           <t>['235.8', '334.1']</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -804,6 +954,16 @@
       <c r="C20" t="n">
         <v>-58</v>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1,450 - 1,508</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -824,6 +984,16 @@
       <c r="C21" t="n">
         <v>78.45</v>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2,199/2,803 </t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -839,6 +1009,16 @@
       <c r="C22" t="n">
         <v>5384</v>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>$2,653.8  +$2,730.2</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -856,6 +1036,12 @@
           <t>['338']</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -875,6 +1061,16 @@
       </c>
       <c r="C24" t="n">
         <v>0</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>(1,895-1,895)/1,895</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -897,6 +1093,16 @@
       <c r="C25" t="n">
         <v>57.86</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>62,899 / (62,899 + 45,812)</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -916,6 +1122,12 @@
       <c r="C26" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>12,958</t>
         </is>
       </c>
     </row>
@@ -938,6 +1150,12 @@
       <c r="C27" t="n">
         <v>-12324</v>
       </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>957-13,281</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -957,6 +1175,12 @@
       <c r="C28" t="n">
         <v>1.93</v>
       </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(1,147,976*9.67)/(881,420*6.53) </t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -972,6 +1196,12 @@
       <c r="C29" t="inlineStr">
         <is>
           <t>['2019']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>locate and analyze Restricted cash included in other assets, noncurrent in row 5</t>
         </is>
       </c>
     </row>
@@ -996,6 +1226,12 @@
       <c r="C30" t="n">
         <v>0.6899999999999999</v>
       </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>(0.82+ 0.71+ 0.55)/3</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1013,6 +1249,8 @@
           <t>['2019', '2018', '2017']</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1032,6 +1270,16 @@
       </c>
       <c r="C32" t="n">
         <v>7.2</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>421.1-413.9</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1054,6 +1302,16 @@
       <c r="C33" t="n">
         <v>0.85</v>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>595,105/701,356</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1071,6 +1329,12 @@
           <t>['6,532']</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1091,6 +1355,16 @@
       <c r="C35" t="n">
         <v>298.08</v>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(207-52)/52 </t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1106,6 +1380,12 @@
       <c r="C36" t="inlineStr">
         <is>
           <t>['2017']</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>$ 14,092&gt;$ 2,526&gt;$ 1,959&gt;$ (724)&gt; $ (11,807)</t>
         </is>
       </c>
     </row>
@@ -1128,6 +1408,16 @@
       <c r="C37" t="n">
         <v>51970</v>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>(50,974 + 52,966) / 2</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1145,6 +1435,12 @@
           <t>4</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Weighted average expected term##Risk-free interest rate##Dividend yield##Volatility</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1160,6 +1456,12 @@
       <c r="C39" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Amortization of right-of-use assets## Interest on lease liabilities</t>
         </is>
       </c>
     </row>
@@ -1180,6 +1482,16 @@
       <c r="C40" t="n">
         <v>85.34</v>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>4,239/4,967</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1196,6 +1508,12 @@
       </c>
       <c r="C41" t="n">
         <v>2810639769</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>3,072,395,752-261,755,983</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -1215,6 +1533,12 @@
       <c r="C42" t="n">
         <v>7</v>
       </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">35/5 </t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1229,6 +1553,16 @@
       </c>
       <c r="C43" t="n">
         <v>0.11</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(230+154+106+304)/751,605 </t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1249,6 +1583,12 @@
       <c r="C44" t="n">
         <v>2248</v>
       </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>(2,248+2,248)/2</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1264,6 +1604,12 @@
       <c r="C45" t="inlineStr">
         <is>
           <t>['2018']</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>$105,959 &gt; $103,884 &gt; $82,253</t>
         </is>
       </c>
     </row>
@@ -1286,6 +1632,16 @@
       <c r="C46" t="n">
         <v>-32.34</v>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>(427,244-631,497)/631,497</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1301,6 +1657,16 @@
       <c r="C47" t="n">
         <v>828035.14</v>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(205,471 / 6.7%) - (176,857 / 7.9%) </t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1318,6 +1684,12 @@
           <t>['197']</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1340,6 +1712,16 @@
       <c r="C49" t="n">
         <v>153.07</v>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(150,777 - 59,578)/59,578 </t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1362,6 +1744,12 @@
           <t>5</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Cost of sales##Selling, general and administrative expenses##Amortization of purchased intangibles##Restructuring costs##Other income</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1382,6 +1770,16 @@
       <c r="C51" t="n">
         <v>0.5</v>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>47.7-47.2</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1402,6 +1800,16 @@
       <c r="C52" t="n">
         <v>10.94</v>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>($14,903-$13,433)/$13,433</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1418,6 +1826,16 @@
       </c>
       <c r="C53" t="n">
         <v>12764.5</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>51,058 / 4</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1437,6 +1855,16 @@
       </c>
       <c r="C54" t="n">
         <v>3.9</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">22.5% - 18.6% </t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1459,6 +1887,16 @@
       <c r="C55" t="n">
         <v>69.70999999999999</v>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">642/921 </t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1476,6 +1914,16 @@
       </c>
       <c r="C56" t="n">
         <v>0.9</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>(1.8 + 0) / 2</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -1499,6 +1947,8 @@
           <t>['Trade payables', 'Accruals', 'Social security and other taxes', 'Other payables']</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1521,6 +1971,16 @@
       <c r="C58" t="n">
         <v>3604.67</v>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>(3,774+3,366+3,674)/3</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1536,6 +1996,12 @@
       <c r="C59" t="inlineStr">
         <is>
           <t>11</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>China##Taiwan##United States##Korea##Europe##Japan##Thailand##Singapore##Malaysia##Philippines##Rest of the World</t>
         </is>
       </c>
     </row>
@@ -1558,6 +2024,12 @@
       <c r="C60" t="n">
         <v>0.8</v>
       </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(3,575+3,041)/8,230 </t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1575,6 +2047,12 @@
           <t>['$259']</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1590,6 +2068,16 @@
       <c r="C62" t="n">
         <v>-3006</v>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- 1,756 + (-1,250) </t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1605,6 +2093,12 @@
       <c r="C63" t="inlineStr">
         <is>
           <t>['2019']</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Find the year with the higher NOL carryover</t>
         </is>
       </c>
     </row>
@@ -1625,6 +2119,16 @@
       </c>
       <c r="C64" t="n">
         <v>14972</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">45,631 + (-30,659) </t>
+        </is>
       </c>
     </row>
     <row r="65">
@@ -1647,6 +2151,16 @@
       <c r="C65" t="n">
         <v>50.69</v>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>77,147 / 152,186</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1667,6 +2181,12 @@
       <c r="C66" t="n">
         <v>887816</v>
       </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>548,788+339,028</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1682,6 +2202,12 @@
       <c r="C67" t="inlineStr">
         <is>
           <t>4</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Maximum##Target##Threshold##Below Threshold</t>
         </is>
       </c>
     </row>
@@ -1706,6 +2232,12 @@
       <c r="C68" t="n">
         <v>2.42</v>
       </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">119,499/49,336 </t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1729,6 +2261,12 @@
           <t>6</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Cost of equipment sold## Other cost of sales## Staff costs## Selling and administrative costs## Traffic Expenses## Repair and maintenance</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1746,6 +2284,12 @@
           <t>3</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>transaction related expenses##integration and transformation costs##special items</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1763,6 +2307,12 @@
           <t>['2017']</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>57,357 &gt; 25,878 &gt; 3,780</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1780,6 +2330,12 @@
           <t>['121.8', '117.7']</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1800,6 +2356,12 @@
       <c r="C73" t="n">
         <v>0.95</v>
       </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 48,866,220/51,297,394</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1819,6 +2381,16 @@
       </c>
       <c r="C74" t="n">
         <v>10160</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1,958 + 8,202 </t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -1842,6 +2414,16 @@
       <c r="C75" t="n">
         <v>0.73</v>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>20,447/28,031</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1859,6 +2441,12 @@
           <t>['2019']</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>5.1&gt;4.0&gt; 3.9</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1874,6 +2462,16 @@
       <c r="C77" t="n">
         <v>8809</v>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4,354 + 4,455 </t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1891,6 +2489,8 @@
           <t>['thereof Germany', 'thereof international']</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1908,6 +2508,12 @@
           <t>['2018']</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>7.8 %&gt;7.4 %</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1923,6 +2529,12 @@
       <c r="C80" t="inlineStr">
         <is>
           <t>['2017']</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>35.0&gt; 21.0</t>
         </is>
       </c>
     </row>
@@ -1943,6 +2555,16 @@
       <c r="C81" t="n">
         <v>121736</v>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">91,132 + 30,604 </t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1960,6 +2582,12 @@
           <t>9</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Server products and cloud services## Office products and cloud services## Windows## Gaming## Search advertising## LinkedIn## Enterprise Services## Devices## Other</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1977,6 +2605,12 @@
           <t>['$3,944']</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1994,6 +2628,16 @@
       </c>
       <c r="C84" t="n">
         <v>70.37</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>1.9/2.7</t>
+        </is>
       </c>
     </row>
     <row r="85">
@@ -2015,6 +2659,16 @@
       <c r="C85" t="n">
         <v>171.09</v>
       </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>(3,657-1,349)/1,349</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2035,6 +2689,16 @@
       <c r="C86" t="n">
         <v>211471.5</v>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>(215,279 + 207,664) / 2</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2049,6 +2713,16 @@
       </c>
       <c r="C87" t="n">
         <v>1072</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>446+378+248</t>
+        </is>
       </c>
     </row>
     <row r="88">
@@ -2069,6 +2743,16 @@
       </c>
       <c r="C88" t="n">
         <v>7.69</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>(28-26)/26</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -2092,6 +2776,16 @@
       <c r="C89" t="n">
         <v>0.63</v>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>(0.9 + 0.8 + 0.2) / 3</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2112,6 +2806,16 @@
       <c r="C90" t="n">
         <v>27.65</v>
       </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(272,098 - 213,159)/213,159 </t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2129,6 +2833,8 @@
           <t>['0.1%']</t>
         </is>
       </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2144,6 +2850,12 @@
       <c r="C92" t="inlineStr">
         <is>
           <t>['2018']</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>24.4% &gt; 23.6% &gt; 23.4%</t>
         </is>
       </c>
     </row>
@@ -2165,6 +2877,12 @@
           <t>['6%', '3%']</t>
         </is>
       </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2182,6 +2900,8 @@
           <t>['$750,000']</t>
         </is>
       </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2199,6 +2919,8 @@
           <t>['7,458,266']</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2221,6 +2943,16 @@
       <c r="C96" t="n">
         <v>4.29</v>
       </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>percent</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>(128.7-123.4)/123.4</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2238,6 +2970,12 @@
       <c r="C97" t="inlineStr">
         <is>
           <t>5</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Other current assets##Property, plant and equipment##Other non-current assets##Debt due within one year##Long-term debt</t>
         </is>
       </c>
     </row>
@@ -2262,6 +3000,8 @@
           <t>['1 April', 'Capital contributions arising from share-based payments', 'Contributions received in relation to share-based payments']</t>
         </is>
       </c>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2282,6 +3022,16 @@
       <c r="C99" t="n">
         <v>45.3</v>
       </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>million</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>180.3-135.0</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2300,6 +3050,12 @@
           <t>['2019']</t>
         </is>
       </c>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>284,967&gt; 245,733&gt; 240,881</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2315,6 +3071,16 @@
       </c>
       <c r="C101" t="n">
         <v>258002</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>thousand</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">($128,706 + $129,296) </t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>